<commit_message>
Schriftliche Akzeptanztests für Registrierung, Login/Logout, Startup erstellen, Startup suchen
</commit_message>
<xml_diff>
--- a/TemplateTestCase v1.6.xlsx
+++ b/TemplateTestCase v1.6.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="133">
   <si>
     <t xml:space="preserve">Simple Test Suite</t>
   </si>
@@ -335,25 +335,7 @@
     <t xml:space="preserve">Student Registrierungs Seite wird angezeigt, es wird nach Daten gefragt</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Vorname, Nachname, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Benutzername, Passwort, Email, Geburtsdatum, Matrikelnr werden eingegeben. Studiengang, Skills werden aus Liste ausgewählt</t>
-    </r>
+    <t xml:space="preserve">Vorname, Nachname, Benutzername, Passwort, Email, Geburtsdatum, Matrikelnr werden eingegeben. Studiengang, Skills werden aus angezeigter Liste ausgewählt</t>
   </si>
   <si>
     <t xml:space="preserve">Eingabefelder sind mit Daten gefüllt</t>
@@ -362,7 +344,7 @@
     <t xml:space="preserve">Button “Registrieren” wird gedrückt</t>
   </si>
   <si>
-    <t xml:space="preserve">Meldung “Nutzer registriert” erscheint, es wird auf die Login Seite navigiert</t>
+    <t xml:space="preserve">Meldung “Nutzer registriert” erscheint, es wird auf die Login Seite navigiert, Login mit den Daten ist jetzt möglich</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamtergebnis:</t>
@@ -388,19 +370,95 @@
   <si>
     <t xml:space="preserve">Fehlermeldung besser mit
 Rotem Hintergrund anzeigen
-Für Sichtbarkeit</t>
+Für Sichtbarkeit → wurde verbessert (18.6.2025)</t>
   </si>
   <si>
     <t xml:space="preserve">Student(“Donald”, “Duck”, “quack”, “Ente123!”, “donald@duck.com”, 08.05.2025, 11112, VWL, Python)</t>
   </si>
   <si>
-    <t xml:space="preserve">Bewerbung schreiben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">falls vorhanden oder anwendbar</t>
+    <t xml:space="preserve">Login und Logout von Benutzer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.06.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_Ä1, registrierter User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startseite von StartupX wird aufgerufen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login-Page wird angezeigt, Login Daten werden angefordert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benutzername “quack” und Passwort “Ente123!” werden in die Login-Felder eingegeben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daten stehen in Eingabefeldern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login Button wird gedrückt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anmeldung ist erfolgreich, Main-Page wird angezeigt, oben rechts steht der Vorname vom User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logout Button oben rechts wird gedrückt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User wird abgemeldet, Session wird geschlossen, es wird wieder die Login-Page angezeigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startup suchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_Ä1, existierendes Startup suchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User loggt sich ein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homepage wird angezeigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigiert zur Seite “Liste von StartUps” durch den Drawer auf der linken Seite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste von StartUp Seite wird angezeigt, zeigt Liste/Tabelle von existierenden Startups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seite öffnet sich, Tabelle mit existierenden Startups wird angezeigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User drückt auf die Suchleiste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suchleiste kann jetzt Suchbegriff bekommen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eingabe von Suchbegriff “EnteGrill”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startup mit Namen “EnteGrill” wird angezeigt, alle anderen StartUps werden herausgefiltert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nur Startup “EnteGrill” wird in Tabelle aufgeführt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro Buchstabe wird die Tabelle
+anhand Suchbegrifft gefiltert,
+Seite aktualisiert sich immer dabei
+(blaue Ladeleiste), vllt wäre
+Ohne Neuladen auch möglich?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doppelklick auf das gesuchte Startup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detaillierte StartUp Sicht wird geöffnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suchbegriff: “EnteGrill”</t>
   </si>
   <si>
     <t xml:space="preserve">Startup erstellen</t>
@@ -424,7 +482,7 @@
     <t xml:space="preserve">Meldung “Startup registriert” erscheint, navigiert zurück zur Startseite</t>
   </si>
   <si>
-    <t xml:space="preserve">Medlung “Nutzer registriert” kommt</t>
+    <t xml:space="preserve">Meldung “Nutzer registriert” kommt</t>
   </si>
   <si>
     <t xml:space="preserve">meh</t>
@@ -796,216 +854,224 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1260,207 +1326,207 @@
   </sheetPr>
   <dimension ref="C3:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="40.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.5"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="12" t="n">
+      <c r="C9" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="12" t="n">
+      <c r="C10" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="12" t="n">
+      <c r="C11" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="12" t="n">
+      <c r="C12" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="13" t="n">
+      <c r="E18" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="22"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="22"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="22"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="22" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="22" t="n">
+      <c r="C25" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1485,1358 +1551,1441 @@
   </sheetPr>
   <dimension ref="B2:H187"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D183" activeCellId="0" sqref="D183"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D101" activeCellId="0" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="37.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="103.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="38.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="103.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.81"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="26" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="33" t="s">
+    <row r="10" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="37" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="n">
+      <c r="B11" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="38"/>
-    </row>
-    <row r="12" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="n">
+      <c r="G11" s="39"/>
+    </row>
+    <row r="12" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="23"/>
+      <c r="F12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="38"/>
-    </row>
-    <row r="13" customFormat="false" ht="85.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="n">
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="13" t="s">
+      <c r="E13" s="23"/>
+      <c r="F13" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="38"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="n">
+      <c r="B14" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="13" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="38"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="39"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="38"/>
+      <c r="G14" s="39"/>
+    </row>
+    <row r="15" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="13"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="39"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="38"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="39"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="38"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="39"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="39"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="38"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="40"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="43"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="44"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="45" t="s">
+      <c r="F21" s="46" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="13" t="s">
+    <row r="27" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="24" t="s">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="26" t="s">
+    <row r="34" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="28" t="s">
+    <row r="35" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="28" t="s">
+    <row r="36" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="28" t="s">
+    <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="46" t="s">
+      <c r="D37" s="47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="30" t="s">
+    <row r="38" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="33" t="s">
+    <row r="41" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E41" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G41" s="36" t="s">
+      <c r="G41" s="37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="12" t="n">
+    <row r="42" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D42" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="38"/>
-    </row>
-    <row r="43" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="12" t="n">
+      <c r="G42" s="39"/>
+    </row>
+    <row r="43" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C43" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="22"/>
-      <c r="F43" s="13" t="s">
+      <c r="E43" s="23"/>
+      <c r="F43" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="38"/>
-    </row>
-    <row r="44" customFormat="false" ht="85.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="12" t="n">
+      <c r="G43" s="39"/>
+    </row>
+    <row r="44" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E44" s="22"/>
-      <c r="F44" s="13" t="s">
+      <c r="E44" s="23"/>
+      <c r="F44" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G44" s="38"/>
-    </row>
-    <row r="45" customFormat="false" ht="51.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="12" t="n">
+      <c r="G44" s="39"/>
+    </row>
+    <row r="45" customFormat="false" ht="64.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C45" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F45" s="13" t="s">
+      <c r="F45" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G45" s="47" t="s">
+      <c r="G45" s="48" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="39"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="38"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="39"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="39"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="38"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="39"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="22"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="38"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="39"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="39"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="38"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="39"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="39"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="38"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="39"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="40"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="43"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="44"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E52" s="44" t="s">
+      <c r="E52" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F52" s="45" t="s">
+      <c r="F52" s="46" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D57" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="13" t="s">
+    <row r="58" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-    </row>
-    <row r="66" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="24" t="s">
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+    </row>
+    <row r="66" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D66" s="25" t="s">
+      <c r="D66" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="26" t="s">
+    <row r="67" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="27" t="s">
+      <c r="D67" s="28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="28" t="s">
+    <row r="68" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="D68" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="28" t="s">
+    <row r="69" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D69" s="29" t="s">
+      <c r="D69" s="30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="28" t="s">
+    <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D70" s="27" t="s">
+      <c r="D70" s="49" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="30" t="s">
+    <row r="71" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="31" t="s">
+      <c r="D71" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="32" t="s">
+      <c r="B73" s="33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="33" t="s">
+    <row r="74" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="34" t="s">
+      <c r="C74" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D74" s="34" t="s">
+      <c r="D74" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E74" s="34" t="s">
+      <c r="E74" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F74" s="35" t="s">
+      <c r="F74" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G74" s="36" t="s">
+      <c r="G74" s="37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="12"/>
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="38"/>
-    </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="12"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="38"/>
-    </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="12"/>
-      <c r="C77" s="37"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="38"/>
-    </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="39"/>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="38"/>
+    <row r="75" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" s="23"/>
+      <c r="F75" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G75" s="39"/>
+    </row>
+    <row r="76" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C76" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E76" s="23"/>
+      <c r="F76" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G76" s="39"/>
+    </row>
+    <row r="77" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C77" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D77" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E77" s="23"/>
+      <c r="F77" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G77" s="39"/>
+    </row>
+    <row r="78" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C78" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D78" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E78" s="23"/>
+      <c r="F78" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G78" s="39"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="39"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="38"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="39"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="39"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="38"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="39"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="39"/>
-      <c r="C81" s="37"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="38"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="38"/>
+      <c r="D81" s="38"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="39"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="39"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="38"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="38"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="39"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="39"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="38"/>
+      <c r="B83" s="40"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="39"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="40"/>
-      <c r="C84" s="41"/>
-      <c r="D84" s="42"/>
-      <c r="E84" s="42"/>
-      <c r="F84" s="19"/>
-      <c r="G84" s="43"/>
+      <c r="B84" s="41"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="43"/>
+      <c r="E84" s="43"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="44"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E85" s="44" t="s">
+      <c r="E85" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F85" s="45"/>
+      <c r="F85" s="46" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="21" t="s">
+      <c r="C90" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D90" s="21" t="s">
+      <c r="D90" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E90" s="21" t="s">
+      <c r="E90" s="22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="13"/>
-      <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
+    <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C91" s="14"/>
+      <c r="D91" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="E91" s="50" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="13"/>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="0"/>
-    </row>
-    <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C97" s="24" t="s">
+      <c r="C94" s="1"/>
+    </row>
+    <row r="97" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C97" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D97" s="25" t="s">
+      <c r="D97" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="26" t="s">
+    <row r="98" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C98" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D98" s="48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C99" s="28" t="s">
+      <c r="D98" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C99" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D99" s="27" t="s">
+      <c r="D99" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C100" s="28" t="s">
+    <row r="100" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C100" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D100" s="29" t="s">
+      <c r="D100" s="30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C101" s="28" t="s">
+    <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C101" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D101" s="46"/>
-    </row>
-    <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="30" t="s">
+      <c r="D101" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C102" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D102" s="31" t="s">
-        <v>55</v>
+      <c r="D102" s="32" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="32" t="s">
+      <c r="B104" s="33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="48.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="33" t="s">
+    <row r="105" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C105" s="34" t="s">
+      <c r="C105" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D105" s="34" t="s">
+      <c r="D105" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E105" s="34" t="s">
+      <c r="E105" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F105" s="35" t="s">
+      <c r="F105" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G105" s="36" t="s">
+      <c r="G105" s="37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="12" t="n">
+    <row r="106" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C106" s="37"/>
-      <c r="D106" s="37"/>
-      <c r="E106" s="22"/>
-      <c r="F106" s="13"/>
-      <c r="G106" s="38"/>
-    </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="12" t="n">
+      <c r="C106" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D106" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E106" s="23"/>
+      <c r="F106" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G106" s="39"/>
+    </row>
+    <row r="107" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C107" s="37"/>
-      <c r="D107" s="37"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="13"/>
-      <c r="G107" s="38"/>
-    </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="12" t="n">
+      <c r="C107" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D107" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="E107" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F107" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G107" s="39"/>
+    </row>
+    <row r="108" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C108" s="37"/>
-      <c r="D108" s="37"/>
-      <c r="E108" s="22"/>
-      <c r="F108" s="13"/>
-      <c r="G108" s="38"/>
-    </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="12" t="n">
+      <c r="C108" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D108" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E108" s="23"/>
+      <c r="F108" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G108" s="39"/>
+    </row>
+    <row r="109" customFormat="false" ht="80.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C109" s="37"/>
-      <c r="D109" s="37"/>
-      <c r="E109" s="22"/>
-      <c r="F109" s="13"/>
-      <c r="G109" s="38"/>
-    </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="12" t="n">
+      <c r="C109" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D109" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="E109" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F109" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G109" s="48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C110" s="37"/>
-      <c r="D110" s="37"/>
-      <c r="E110" s="22"/>
-      <c r="F110" s="13"/>
-      <c r="G110" s="38"/>
+      <c r="C110" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D110" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E110" s="23"/>
+      <c r="F110" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G110" s="39"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="39"/>
-      <c r="C111" s="37"/>
-      <c r="D111" s="37"/>
-      <c r="E111" s="22"/>
-      <c r="F111" s="13"/>
-      <c r="G111" s="38"/>
+      <c r="B111" s="40"/>
+      <c r="C111" s="38"/>
+      <c r="D111" s="38"/>
+      <c r="E111" s="23"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="39"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="39"/>
-      <c r="C112" s="37"/>
-      <c r="D112" s="37"/>
-      <c r="E112" s="22"/>
-      <c r="F112" s="13"/>
-      <c r="G112" s="38"/>
+      <c r="B112" s="40"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="38"/>
+      <c r="E112" s="23"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="39"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="39"/>
-      <c r="C113" s="37"/>
-      <c r="D113" s="37"/>
-      <c r="E113" s="22"/>
-      <c r="F113" s="13"/>
-      <c r="G113" s="38"/>
+      <c r="B113" s="40"/>
+      <c r="C113" s="38"/>
+      <c r="D113" s="38"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="39"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="39"/>
-      <c r="C114" s="37"/>
-      <c r="D114" s="37"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="13"/>
-      <c r="G114" s="38"/>
+      <c r="B114" s="40"/>
+      <c r="C114" s="38"/>
+      <c r="D114" s="38"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="14"/>
+      <c r="G114" s="39"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="40"/>
-      <c r="C115" s="41"/>
-      <c r="D115" s="42"/>
-      <c r="E115" s="42"/>
-      <c r="F115" s="19"/>
-      <c r="G115" s="43"/>
+      <c r="B115" s="41"/>
+      <c r="C115" s="42"/>
+      <c r="D115" s="43"/>
+      <c r="E115" s="43"/>
+      <c r="F115" s="20"/>
+      <c r="G115" s="44"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E116" s="44" t="s">
+      <c r="E116" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F116" s="45"/>
+      <c r="F116" s="46" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="6" t="s">
+      <c r="C119" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="21" t="s">
+      <c r="C121" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D121" s="21" t="s">
+      <c r="D121" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E121" s="21" t="s">
+      <c r="E121" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="13"/>
-      <c r="D122" s="46"/>
-      <c r="E122" s="13"/>
+      <c r="C122" s="14"/>
+      <c r="D122" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E122" s="51" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C123" s="13"/>
-      <c r="D123" s="13"/>
-      <c r="E123" s="13"/>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C124" s="13"/>
-      <c r="D124" s="13"/>
-      <c r="E124" s="13"/>
-    </row>
-    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C129" s="24" t="s">
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+    </row>
+    <row r="129" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C129" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D129" s="25" t="s">
+      <c r="D129" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C130" s="26" t="s">
+    <row r="130" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C130" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D130" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C131" s="28" t="s">
+      <c r="D130" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D131" s="27" t="s">
+      <c r="D131" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="28" t="s">
+    <row r="132" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C132" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D132" s="29" t="s">
+      <c r="D132" s="30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C133" s="28" t="s">
+    <row r="133" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C133" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D133" s="46" t="s">
+      <c r="D133" s="47" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="30" t="s">
+    <row r="134" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D134" s="31" t="s">
+      <c r="D134" s="32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="18.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B136" s="32" t="s">
+      <c r="B136" s="33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="38.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B137" s="33" t="s">
+      <c r="B137" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C137" s="34" t="s">
+      <c r="C137" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D137" s="34" t="s">
+      <c r="D137" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E137" s="34" t="s">
+      <c r="E137" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F137" s="35" t="s">
+      <c r="F137" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G137" s="36" t="s">
+      <c r="G137" s="37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="12" t="n">
+    <row r="138" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C138" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D138" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E138" s="22"/>
-      <c r="F138" s="13" t="s">
+      <c r="C138" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D138" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E138" s="23"/>
+      <c r="F138" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G138" s="38"/>
-    </row>
-    <row r="139" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="12" t="n">
+      <c r="G138" s="39"/>
+    </row>
+    <row r="139" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C139" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="D139" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E139" s="22"/>
-      <c r="F139" s="13" t="s">
+      <c r="C139" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D139" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E139" s="23"/>
+      <c r="F139" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G139" s="38"/>
-    </row>
-    <row r="140" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="12" t="n">
+      <c r="G139" s="39"/>
+    </row>
+    <row r="140" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C140" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="D140" s="37" t="s">
+      <c r="C140" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D140" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E140" s="22"/>
-      <c r="F140" s="13" t="s">
+      <c r="E140" s="23"/>
+      <c r="F140" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G140" s="38"/>
+      <c r="G140" s="39"/>
     </row>
     <row r="141" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="12" t="n">
+      <c r="B141" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C141" s="37" t="s">
+      <c r="C141" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D141" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E141" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F141" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G141" s="38" t="s">
-        <v>72</v>
+      <c r="D141" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E141" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F141" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G141" s="39" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="39"/>
-      <c r="C142" s="37"/>
-      <c r="D142" s="37"/>
-      <c r="E142" s="22"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="38"/>
+      <c r="B142" s="40"/>
+      <c r="C142" s="38"/>
+      <c r="D142" s="38"/>
+      <c r="E142" s="23"/>
+      <c r="F142" s="14"/>
+      <c r="G142" s="39"/>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="39"/>
-      <c r="C143" s="37"/>
-      <c r="D143" s="37"/>
-      <c r="E143" s="22"/>
-      <c r="F143" s="13"/>
-      <c r="G143" s="38"/>
+      <c r="B143" s="40"/>
+      <c r="C143" s="38"/>
+      <c r="D143" s="38"/>
+      <c r="E143" s="23"/>
+      <c r="F143" s="14"/>
+      <c r="G143" s="39"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B144" s="39"/>
-      <c r="C144" s="37"/>
-      <c r="D144" s="37"/>
-      <c r="E144" s="22"/>
-      <c r="F144" s="13"/>
-      <c r="G144" s="38"/>
+      <c r="B144" s="40"/>
+      <c r="C144" s="38"/>
+      <c r="D144" s="38"/>
+      <c r="E144" s="23"/>
+      <c r="F144" s="14"/>
+      <c r="G144" s="39"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="39"/>
-      <c r="C145" s="37"/>
-      <c r="D145" s="37"/>
-      <c r="E145" s="22"/>
-      <c r="F145" s="13"/>
-      <c r="G145" s="38"/>
+      <c r="B145" s="40"/>
+      <c r="C145" s="38"/>
+      <c r="D145" s="38"/>
+      <c r="E145" s="23"/>
+      <c r="F145" s="14"/>
+      <c r="G145" s="39"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="39"/>
-      <c r="C146" s="37"/>
-      <c r="D146" s="37"/>
-      <c r="E146" s="22"/>
-      <c r="F146" s="13"/>
-      <c r="G146" s="38"/>
+      <c r="B146" s="40"/>
+      <c r="C146" s="38"/>
+      <c r="D146" s="38"/>
+      <c r="E146" s="23"/>
+      <c r="F146" s="14"/>
+      <c r="G146" s="39"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="40"/>
-      <c r="C147" s="41"/>
-      <c r="D147" s="42"/>
-      <c r="E147" s="42"/>
-      <c r="F147" s="19"/>
-      <c r="G147" s="43"/>
+      <c r="B147" s="41"/>
+      <c r="C147" s="42"/>
+      <c r="D147" s="43"/>
+      <c r="E147" s="43"/>
+      <c r="F147" s="20"/>
+      <c r="G147" s="44"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E148" s="44" t="s">
+      <c r="E148" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F148" s="45" t="s">
-        <v>71</v>
+      <c r="F148" s="46" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="6" t="s">
+      <c r="C151" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C153" s="21" t="s">
+      <c r="C153" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D153" s="21" t="s">
+      <c r="D153" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E153" s="21" t="s">
+      <c r="E153" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C154" s="13"/>
-      <c r="D154" s="13" t="s">
+      <c r="C154" s="14"/>
+      <c r="D154" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E154" s="13" t="s">
-        <v>73</v>
+      <c r="E154" s="14" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C155" s="13"/>
-      <c r="D155" s="13"/>
-      <c r="E155" s="13"/>
+      <c r="C155" s="14"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C156" s="13"/>
-      <c r="D156" s="13"/>
-      <c r="E156" s="13"/>
+      <c r="C156" s="14"/>
+      <c r="D156" s="14"/>
+      <c r="E156" s="14"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C157" s="0"/>
-    </row>
-    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="24" t="s">
+      <c r="C157" s="1"/>
+    </row>
+    <row r="160" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C160" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D160" s="25" t="s">
+      <c r="D160" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="26" t="s">
+    <row r="161" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C161" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D161" s="48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="28" t="s">
+      <c r="D161" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C162" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D162" s="27" t="s">
+      <c r="D162" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="28" t="s">
+    <row r="163" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C163" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D163" s="29" t="s">
+      <c r="D163" s="30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="18.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C164" s="28" t="s">
+    <row r="164" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C164" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D164" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C165" s="30" t="s">
+      <c r="D164" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C165" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D165" s="31" t="s">
+      <c r="D165" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="167" customFormat="false" ht="24.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B167" s="32" t="s">
+      <c r="B167" s="33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B168" s="33" t="s">
+      <c r="B168" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C168" s="34" t="s">
+      <c r="C168" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D168" s="34" t="s">
+      <c r="D168" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E168" s="34" t="s">
+      <c r="E168" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F168" s="35" t="s">
+      <c r="F168" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G168" s="36" t="s">
+      <c r="G168" s="37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="18.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="12" t="n">
+    <row r="169" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C169" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D169" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E169" s="22"/>
-      <c r="F169" s="13" t="s">
+      <c r="C169" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D169" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E169" s="23"/>
+      <c r="F169" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G169" s="38"/>
-    </row>
-    <row r="170" customFormat="false" ht="35.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B170" s="12" t="n">
+      <c r="G169" s="39"/>
+    </row>
+    <row r="170" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B170" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C170" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="D170" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E170" s="22"/>
-      <c r="F170" s="13" t="s">
+      <c r="C170" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D170" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E170" s="23"/>
+      <c r="F170" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G170" s="38"/>
+      <c r="G170" s="39"/>
     </row>
     <row r="171" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B171" s="12" t="n">
+      <c r="B171" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C171" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="D171" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="E171" s="22"/>
-      <c r="F171" s="13" t="s">
+      <c r="C171" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D171" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="E171" s="23"/>
+      <c r="F171" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G171" s="38"/>
+      <c r="G171" s="39"/>
     </row>
     <row r="172" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B172" s="12" t="n">
+      <c r="B172" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C172" s="37" t="s">
+      <c r="C172" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D172" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E172" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F172" s="13" t="s">
+      <c r="D172" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E172" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F172" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G172" s="38" t="s">
-        <v>78</v>
+      <c r="G172" s="39" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="39"/>
-      <c r="C173" s="37"/>
-      <c r="D173" s="37"/>
-      <c r="E173" s="22"/>
-      <c r="F173" s="13"/>
-      <c r="G173" s="38"/>
+      <c r="B173" s="40"/>
+      <c r="C173" s="38"/>
+      <c r="D173" s="38"/>
+      <c r="E173" s="23"/>
+      <c r="F173" s="14"/>
+      <c r="G173" s="39"/>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="39"/>
-      <c r="C174" s="37"/>
-      <c r="D174" s="37"/>
-      <c r="E174" s="22"/>
-      <c r="F174" s="13"/>
-      <c r="G174" s="38"/>
+      <c r="B174" s="40"/>
+      <c r="C174" s="38"/>
+      <c r="D174" s="38"/>
+      <c r="E174" s="23"/>
+      <c r="F174" s="14"/>
+      <c r="G174" s="39"/>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="39"/>
-      <c r="C175" s="37"/>
-      <c r="D175" s="37"/>
-      <c r="E175" s="22"/>
-      <c r="F175" s="13"/>
-      <c r="G175" s="38"/>
+      <c r="B175" s="40"/>
+      <c r="C175" s="38"/>
+      <c r="D175" s="38"/>
+      <c r="E175" s="23"/>
+      <c r="F175" s="14"/>
+      <c r="G175" s="39"/>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B176" s="39"/>
-      <c r="C176" s="37"/>
-      <c r="D176" s="37"/>
-      <c r="E176" s="22"/>
-      <c r="F176" s="13"/>
-      <c r="G176" s="38"/>
+      <c r="B176" s="40"/>
+      <c r="C176" s="38"/>
+      <c r="D176" s="38"/>
+      <c r="E176" s="23"/>
+      <c r="F176" s="14"/>
+      <c r="G176" s="39"/>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B177" s="39"/>
-      <c r="C177" s="37"/>
-      <c r="D177" s="37"/>
-      <c r="E177" s="22"/>
-      <c r="F177" s="13"/>
-      <c r="G177" s="38"/>
+      <c r="B177" s="40"/>
+      <c r="C177" s="38"/>
+      <c r="D177" s="38"/>
+      <c r="E177" s="23"/>
+      <c r="F177" s="14"/>
+      <c r="G177" s="39"/>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B178" s="40"/>
-      <c r="C178" s="41"/>
-      <c r="D178" s="42"/>
-      <c r="E178" s="42"/>
-      <c r="F178" s="19"/>
-      <c r="G178" s="43"/>
+      <c r="B178" s="41"/>
+      <c r="C178" s="42"/>
+      <c r="D178" s="43"/>
+      <c r="E178" s="43"/>
+      <c r="F178" s="20"/>
+      <c r="G178" s="44"/>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E179" s="44" t="s">
+      <c r="E179" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F179" s="45" t="s">
+      <c r="F179" s="46" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C182" s="6" t="s">
+      <c r="C182" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="21" t="s">
+      <c r="C184" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D184" s="21" t="s">
+      <c r="D184" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E184" s="21" t="s">
+      <c r="E184" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C185" s="13"/>
-      <c r="D185" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E185" s="13" t="s">
-        <v>79</v>
+      <c r="C185" s="14"/>
+      <c r="D185" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E185" s="14" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="13"/>
-      <c r="D186" s="13"/>
-      <c r="E186" s="13"/>
+      <c r="C186" s="14"/>
+      <c r="D186" s="14"/>
+      <c r="E186" s="14"/>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C187" s="13"/>
-      <c r="D187" s="13"/>
-      <c r="E187" s="13"/>
+      <c r="C187" s="14"/>
+      <c r="D187" s="14"/>
+      <c r="E187" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E27" r:id="rId1" display="donald@duck.com"/>
-    <hyperlink ref="E58" r:id="rId2" display="donald@duck.com"/>
+    <hyperlink ref="E27" r:id="rId1" display="Student(“Donald”, “Duck”, “quack”, “Ente123!”, “donald@duck.com”, 06.03.2025, 11111, Informatik, Photoshop)"/>
+    <hyperlink ref="E58" r:id="rId2" display="Student(“Donald”, “Duck”, “quack”, “Ente123!”, “donald@duck.com”, 08.05.2025, 11112, VWL, Python)"/>
+    <hyperlink ref="E91" r:id="rId3" display="Student(“Donald”, “Duck”, “quack”, “Ente123!”, “donald@duck.com”, 06.03.2025, 11111, Informatik, Photoshop)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2855,228 +3004,228 @@
   </sheetPr>
   <dimension ref="B3:G29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="46.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="46.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.5"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="49" t="s">
-        <v>80</v>
+      <c r="D3" s="52" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>81</v>
+      <c r="D4" s="47" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="50" t="s">
-        <v>82</v>
+      <c r="D5" s="47" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="51" t="n">
+      <c r="D6" s="53" t="n">
         <v>43927</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>83</v>
+      <c r="D7" s="47" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="54" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="37" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="n">
+      <c r="B12" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="38"/>
+      <c r="C12" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="39"/>
     </row>
     <row r="13" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="n">
+      <c r="B13" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="38"/>
+      <c r="C13" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="23"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="n">
+      <c r="B14" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="38"/>
+      <c r="C14" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="38"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="39"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="38"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="39"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="38"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="39"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="39"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="38"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="39"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="38"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="39"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="43"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="45"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>91</v>
+      <c r="C28" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3096,265 +3245,265 @@
   </sheetPr>
   <dimension ref="B3:G30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="23" width="46.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="46.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.5"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="49" t="s">
-        <v>92</v>
+      <c r="D3" s="52" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>93</v>
+      <c r="D4" s="47" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="50" t="s">
-        <v>82</v>
+      <c r="D5" s="47" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="51" t="n">
+      <c r="D6" s="53" t="n">
         <v>43927</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>94</v>
+      <c r="D7" s="47" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="54" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="37" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="n">
+      <c r="B12" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" s="13" t="s">
+      <c r="C12" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="38"/>
+      <c r="G12" s="39"/>
     </row>
     <row r="13" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="n">
+      <c r="B13" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="13" t="s">
+      <c r="C13" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="23"/>
+      <c r="F13" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="38"/>
+      <c r="G13" s="39"/>
     </row>
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12" t="n">
+      <c r="B14" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="13" t="s">
+      <c r="C14" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="38"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="n">
+      <c r="B15" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="C15" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="13" t="s">
+      <c r="C15" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="38"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="n">
+      <c r="B16" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="C16" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="13" t="s">
+      <c r="C16" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="38"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="39"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="38"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="39"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="39"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="39"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="38"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="39"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="38"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="39"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="43"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="45" t="s">
+      <c r="F22" s="46" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>106</v>
+      <c r="C28" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>108</v>
+      <c r="C29" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>